<commit_message>
create testView(but not complete)
</commit_message>
<xml_diff>
--- a/work-record/作業管理表（先崎）.xlsx
+++ b/work-record/作業管理表（先崎）.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>日付</t>
     <rPh sb="0" eb="2">
@@ -272,6 +272,27 @@
     <t>同上</t>
     <rPh sb="0" eb="2">
       <t>ドウジョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ビューをコンソールで表示</t>
+    <rPh sb="10" eb="12">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>3時間半</t>
+    <rPh sb="1" eb="4">
+      <t>ジカンハン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>50行ぐらい</t>
+    <rPh sb="2" eb="3">
+      <t>ギョウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -640,7 +661,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
@@ -801,6 +822,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="1">
+        <v>42713</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>